<commit_message>
Added ->display only valid sets
</commit_message>
<xml_diff>
--- a/Graph1.xlsx
+++ b/Graph1.xlsx
@@ -11,6 +11,443 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="144">
+  <si>
+    <t>0.1935</t>
+  </si>
+  <si>
+    <t>0.114797</t>
+  </si>
+  <si>
+    <t>4.023497</t>
+  </si>
+  <si>
+    <t>0.1560</t>
+  </si>
+  <si>
+    <t>0.140329</t>
+  </si>
+  <si>
+    <t>3.291529</t>
+  </si>
+  <si>
+    <t>0.1427</t>
+  </si>
+  <si>
+    <t>0.14682</t>
+  </si>
+  <si>
+    <t>3.02936</t>
+  </si>
+  <si>
+    <t>0.1363</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>2.75326</t>
+  </si>
+  <si>
+    <t>0.1370</t>
+  </si>
+  <si>
+    <t>0.155484</t>
+  </si>
+  <si>
+    <t>2.922884</t>
+  </si>
+  <si>
+    <t>0.1477</t>
+  </si>
+  <si>
+    <t>0.12909</t>
+  </si>
+  <si>
+    <t>3.11263</t>
+  </si>
+  <si>
+    <t>0.1071</t>
+  </si>
+  <si>
+    <t>0.161691</t>
+  </si>
+  <si>
+    <t>2.325111</t>
+  </si>
+  <si>
+    <t>0.0962</t>
+  </si>
+  <si>
+    <t>0.154496</t>
+  </si>
+  <si>
+    <t>2.097736</t>
+  </si>
+  <si>
+    <t>0.0907</t>
+  </si>
+  <si>
+    <t>0.180686</t>
+  </si>
+  <si>
+    <t>2.012826</t>
+  </si>
+  <si>
+    <t>0.0886</t>
+  </si>
+  <si>
+    <t>0.176515</t>
+  </si>
+  <si>
+    <t>1.966235</t>
+  </si>
+  <si>
+    <t>0.1002</t>
+  </si>
+  <si>
+    <t>0.147005</t>
+  </si>
+  <si>
+    <t>2.171045</t>
+  </si>
+  <si>
+    <t>0.0753</t>
+  </si>
+  <si>
+    <t>0.181131</t>
+  </si>
+  <si>
+    <t>1.702191</t>
+  </si>
+  <si>
+    <t>0.0599</t>
+  </si>
+  <si>
+    <t>0.185685</t>
+  </si>
+  <si>
+    <t>1.395665</t>
+  </si>
+  <si>
+    <t>0.0536</t>
+  </si>
+  <si>
+    <t>0.189065</t>
+  </si>
+  <si>
+    <t>1.271785</t>
+  </si>
+  <si>
+    <t>0.0495</t>
+  </si>
+  <si>
+    <t>0.182948</t>
+  </si>
+  <si>
+    <t>1.182848</t>
+  </si>
+  <si>
+    <t>0.0670</t>
+  </si>
+  <si>
+    <t>0.16383</t>
+  </si>
+  <si>
+    <t>1.51723</t>
+  </si>
+  <si>
+    <t>0.0473</t>
+  </si>
+  <si>
+    <t>0.194195</t>
+  </si>
+  <si>
+    <t>1.149655</t>
+  </si>
+  <si>
+    <t>0.0425</t>
+  </si>
+  <si>
+    <t>0.211173</t>
+  </si>
+  <si>
+    <t>1.069673</t>
+  </si>
+  <si>
+    <t>0.0395</t>
+  </si>
+  <si>
+    <t>0.212911</t>
+  </si>
+  <si>
+    <t>1.010811</t>
+  </si>
+  <si>
+    <t>0.0391</t>
+  </si>
+  <si>
+    <t>0.198581</t>
+  </si>
+  <si>
+    <t>0.988401</t>
+  </si>
+  <si>
+    <t>0.0461</t>
+  </si>
+  <si>
+    <t>0.198417</t>
+  </si>
+  <si>
+    <t>1.129637</t>
+  </si>
+  <si>
+    <t>0.0338</t>
+  </si>
+  <si>
+    <t>0.223917</t>
+  </si>
+  <si>
+    <t>0.906677</t>
+  </si>
+  <si>
+    <t>0.0283</t>
+  </si>
+  <si>
+    <t>0.233936</t>
+  </si>
+  <si>
+    <t>0.805596</t>
+  </si>
+  <si>
+    <t>0.0277</t>
+  </si>
+  <si>
+    <t>0.254354</t>
+  </si>
+  <si>
+    <t>0.813894</t>
+  </si>
+  <si>
+    <t>0.0263</t>
+  </si>
+  <si>
+    <t>0.205608</t>
+  </si>
+  <si>
+    <t>0.736868</t>
+  </si>
+  <si>
+    <t>0.0377</t>
+  </si>
+  <si>
+    <t>0.233353</t>
+  </si>
+  <si>
+    <t>0.994893</t>
+  </si>
+  <si>
+    <t>0.0288</t>
+  </si>
+  <si>
+    <t>0.262446</t>
+  </si>
+  <si>
+    <t>0.844206</t>
+  </si>
+  <si>
+    <t>0.0264</t>
+  </si>
+  <si>
+    <t>0.27125</t>
+  </si>
+  <si>
+    <t>0.80453</t>
+  </si>
+  <si>
+    <t>0.0262</t>
+  </si>
+  <si>
+    <t>0.288511</t>
+  </si>
+  <si>
+    <t>0.817751</t>
+  </si>
+  <si>
+    <t>0.22474</t>
+  </si>
+  <si>
+    <t>0.75398</t>
+  </si>
+  <si>
+    <t>0.0329</t>
+  </si>
+  <si>
+    <t>0.294627</t>
+  </si>
+  <si>
+    <t>0.959207</t>
+  </si>
+  <si>
+    <t>0.0271</t>
+  </si>
+  <si>
+    <t>0.300727</t>
+  </si>
+  <si>
+    <t>0.848147</t>
+  </si>
+  <si>
+    <t>0.0259</t>
+  </si>
+  <si>
+    <t>0.319481</t>
+  </si>
+  <si>
+    <t>0.842661</t>
+  </si>
+  <si>
+    <t>0.341213</t>
+  </si>
+  <si>
+    <t>0.864393</t>
+  </si>
+  <si>
+    <t>0.0258</t>
+  </si>
+  <si>
+    <t>0.276281</t>
+  </si>
+  <si>
+    <t>0.797441</t>
+  </si>
+  <si>
+    <t>0.0323</t>
+  </si>
+  <si>
+    <t>0.3668</t>
+  </si>
+  <si>
+    <t>1.01926</t>
+  </si>
+  <si>
+    <t>0.374603</t>
+  </si>
+  <si>
+    <t>0.897783</t>
+  </si>
+  <si>
+    <t>0.38028</t>
+  </si>
+  <si>
+    <t>0.90144</t>
+  </si>
+  <si>
+    <t>0.401236</t>
+  </si>
+  <si>
+    <t>0.922396</t>
+  </si>
+  <si>
+    <t>0.322486</t>
+  </si>
+  <si>
+    <t>0.843646</t>
+  </si>
+  <si>
+    <t>0.443812</t>
+  </si>
+  <si>
+    <t>0.964972</t>
+  </si>
+  <si>
+    <t>0.445929</t>
+  </si>
+  <si>
+    <t>0.967089</t>
+  </si>
+  <si>
+    <t>0.457685</t>
+  </si>
+  <si>
+    <t>0.978845</t>
+  </si>
+  <si>
+    <t>0.458925</t>
+  </si>
+  <si>
+    <t>0.980085</t>
+  </si>
+  <si>
+    <t>0.396009</t>
+  </si>
+  <si>
+    <t>0.917169</t>
+  </si>
+  <si>
+    <t>0.563451</t>
+  </si>
+  <si>
+    <t>1.084611</t>
+  </si>
+  <si>
+    <t>0.567744</t>
+  </si>
+  <si>
+    <t>1.088904</t>
+  </si>
+  <si>
+    <t>0.564418</t>
+  </si>
+  <si>
+    <t>1.085578</t>
+  </si>
+  <si>
+    <t>0.578177</t>
+  </si>
+  <si>
+    <t>1.099337</t>
+  </si>
+  <si>
+    <t>0.475728</t>
+  </si>
+  <si>
+    <t>0.996888</t>
+  </si>
+  <si>
+    <t>0.69938</t>
+  </si>
+  <si>
+    <t>1.22054</t>
+  </si>
+  <si>
+    <t>0.706046</t>
+  </si>
+  <si>
+    <t>1.227206</t>
+  </si>
+  <si>
+    <t>0.699607</t>
+  </si>
+  <si>
+    <t>1.220767</t>
+  </si>
+  <si>
+    <t>0.705819</t>
+  </si>
+  <si>
+    <t>1.226979</t>
+  </si>
+  <si>
+    <t>0.588474</t>
+  </si>
+  <si>
+    <t>1.109634</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +777,948 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1">
+        <v>1024</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1024</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1024</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1024</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1024</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>2048</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2048</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2048</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2048</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2048</v>
+      </c>
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>4096</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>4096</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>4096</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>4096</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>4096</v>
+      </c>
+      <c r="B15">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>8192</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>8192</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>8192</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>8192</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>8192</v>
+      </c>
+      <c r="B20">
+        <v>256</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>16384</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>16384</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>16384</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>16384</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>16384</v>
+      </c>
+      <c r="B25">
+        <v>512</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>32768</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>32768</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>32768</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>32768</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>32768</v>
+      </c>
+      <c r="B30">
+        <v>1024</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>65536</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>65536</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>65536</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>65536</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>65536</v>
+      </c>
+      <c r="B35">
+        <v>2048</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>131072</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>131072</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
+        <v>106</v>
+      </c>
+      <c r="E37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>131072</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>131072</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>131072</v>
+      </c>
+      <c r="B40">
+        <v>4096</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>262144</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>262144</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>262144</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>262144</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>262144</v>
+      </c>
+      <c r="B45">
+        <v>8192</v>
+      </c>
+      <c r="C45" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>524288</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>524288</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>524288</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>524288</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>524288</v>
+      </c>
+      <c r="B50">
+        <v>16384</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>1048576</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>1048576</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>1048576</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>1048576</v>
+      </c>
+      <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>1048576</v>
+      </c>
+      <c r="B55">
+        <v>32768</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>